<commit_message>
For Bug Fixes Reposrted By Daniel
</commit_message>
<xml_diff>
--- a/NtierMvc/App_Data/Documents/Excel/ProductPerformance.xlsx
+++ b/NtierMvc/App_Data/Documents/Excel/ProductPerformance.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepak\Downloads\C#\NtierMvc\App_Data\Documents\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DF56CC-E7B6-45BB-90B8-6B2940D167B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19800" windowHeight="7665"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Report!$A$3:$D$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Report!$A$3:$D$13</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
@@ -62,7 +68,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -372,23 +378,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -399,17 +399,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -420,6 +422,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -468,7 +473,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -501,9 +506,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -536,6 +558,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -711,14 +750,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -763,16 +802,16 @@
       <c r="D4" s="13"/>
     </row>
     <row r="5" spans="1:4" ht="50.25" customHeight="1">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="20" t="s">
         <v>7</v>
       </c>
     </row>
@@ -782,57 +821,59 @@
       <c r="C6" s="15"/>
       <c r="D6" s="16"/>
     </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" ht="41.25" customHeight="1">
+    <row r="7" spans="1:4" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
     </row>
-    <row r="8" spans="1:4" ht="113.25" customHeight="1">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:4" s="1" customFormat="1" ht="41.25" customHeight="1">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:4" ht="113.25" customHeight="1">
+      <c r="A9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
-    </row>
-    <row r="9" spans="1:4" ht="69.75" customHeight="1">
-      <c r="A9" s="20" t="s">
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
+    </row>
+    <row r="10" spans="1:4" ht="69.75" customHeight="1">
+      <c r="A10" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="22"/>
-    </row>
-    <row r="10" spans="1:4" ht="60" customHeight="1">
-      <c r="A10" s="20" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="29"/>
+    </row>
+    <row r="11" spans="1:4" ht="60" customHeight="1">
+      <c r="A11" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
-    </row>
-    <row r="11" spans="1:4" ht="78.75" customHeight="1">
-      <c r="A11" s="20" t="s">
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="29"/>
+    </row>
+    <row r="12" spans="1:4" ht="78.75" customHeight="1">
+      <c r="A12" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
-    </row>
-    <row r="12" spans="1:4" ht="52.5" customHeight="1">
-      <c r="A12" s="23"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="29"/>
+    </row>
+    <row r="13" spans="1:4" ht="52.5" customHeight="1">
+      <c r="A13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A12:D12"/>
+  <mergeCells count="1">
+    <mergeCell ref="A13:D13"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992126" right="0.196850393700787" top="1.2992125984252001" bottom="0.196850393700787" header="0.196850393700787" footer="0.196850393700787"/>

</xml_diff>

<commit_message>
Template and Bugs Update
</commit_message>
<xml_diff>
--- a/NtierMvc/App_Data/Documents/Excel/ProductPerformance.xlsx
+++ b/NtierMvc/App_Data/Documents/Excel/ProductPerformance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepak\Downloads\C#\NtierMvc\App_Data\Documents\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DF56CC-E7B6-45BB-90B8-6B2940D167B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADA5C16-390C-4706-81DF-5D620295615A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Report" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Report!$A$3:$D$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Report!$A$3:$D$16</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>MOT/F/SM/07 REV. 02</t>
   </si>
@@ -49,13 +49,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t xml:space="preserve">
-We want to confirm that your shipment of supplied above products have met our expectations completely. 
-Product quality and performance of the product found best along with on time response and delivery time from your company.
-Furthermore, we expect to continue good results with application of your manufactured products on our oil fields.
-</t>
-  </si>
-  <si>
     <t>Customer Comments:</t>
   </si>
   <si>
@@ -63,6 +56,18 @@
   </si>
   <si>
     <t>Customer Seal:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We want to confirm that your shipment of supplied above products have met our expectations completely. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product quality and performance of the product found best along with on time response and delivery time from </t>
+  </si>
+  <si>
+    <t>your company.</t>
+  </si>
+  <si>
+    <t>Furthermore, we expect to continue good results with application of your manufactured products on our oil fields.</t>
   </si>
 </sst>
 </file>
@@ -133,7 +138,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -326,11 +331,126 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -351,15 +471,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -390,27 +501,64 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -754,10 +902,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -769,7 +917,7 @@
     <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -777,7 +925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="73.5" customHeight="1">
+    <row r="2" spans="1:4" ht="73.5" customHeight="1" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -786,95 +934,116 @@
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" ht="34.5" customHeight="1">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="31"/>
     </row>
     <row r="4" spans="1:4" ht="39" customHeight="1">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:4" ht="50.25" customHeight="1">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="17" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13"/>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" ht="41.25" customHeight="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-    </row>
-    <row r="9" spans="1:4" ht="113.25" customHeight="1">
-      <c r="A9" s="24" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="23"/>
+    </row>
+    <row r="9" spans="1:4" ht="27" customHeight="1">
+      <c r="A9" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="36"/>
+    </row>
+    <row r="10" spans="1:4" ht="23.25" customHeight="1">
+      <c r="A10" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="33"/>
+    </row>
+    <row r="11" spans="1:4" ht="21.75" customHeight="1">
+      <c r="A11" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="33"/>
+    </row>
+    <row r="12" spans="1:4" ht="23.25" customHeight="1">
+      <c r="A12" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="34"/>
+    </row>
+    <row r="13" spans="1:4" ht="69.75" customHeight="1">
+      <c r="A13" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="26"/>
-    </row>
-    <row r="10" spans="1:4" ht="69.75" customHeight="1">
-      <c r="A10" s="27" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+    </row>
+    <row r="14" spans="1:4" ht="60" customHeight="1">
+      <c r="A14" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="29"/>
-    </row>
-    <row r="11" spans="1:4" ht="60" customHeight="1">
-      <c r="A11" s="27" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+    </row>
+    <row r="15" spans="1:4" ht="78.75" customHeight="1">
+      <c r="A15" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="29"/>
-    </row>
-    <row r="12" spans="1:4" ht="78.75" customHeight="1">
-      <c r="A12" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
-    </row>
-    <row r="13" spans="1:4" ht="52.5" customHeight="1">
-      <c r="A13" s="21"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+    </row>
+    <row r="16" spans="1:4" ht="52.5" customHeight="1" thickBot="1">
+      <c r="A16" s="26"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A13:D13"/>
-  </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992126" right="0.196850393700787" top="1.2992125984252001" bottom="0.196850393700787" header="0.196850393700787" footer="0.196850393700787"/>
   <pageSetup paperSize="9" scale="86" fitToHeight="1000" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>